<commit_message>
sql scripts sponsor created
</commit_message>
<xml_diff>
--- a/Source/Navn og passord.xlsx
+++ b/Source/Navn og passord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/557edc836ab4960f/Dokumenter/Databaser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MaineBoat\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{3FCF2569-5BF1-4099-A278-053608C4E6ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C20D2B-3D3A-4F18-8DFC-17EA200E0480}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18120" yWindow="450" windowWidth="10395" windowHeight="7800" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,18 +496,18 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
     <col min="11" max="11" width="18.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Skiftet Admin, selskap og sponsor til ny server
</commit_message>
<xml_diff>
--- a/Source/Navn og passord.xlsx
+++ b/Source/Navn og passord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MaineBoat\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C20D2B-3D3A-4F18-8DFC-17EA200E0480}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F198B91A-5DBD-45C3-B998-09FF1B1C1178}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
   <si>
     <t>Eier</t>
   </si>
@@ -136,19 +136,76 @@
   </si>
   <si>
     <t>105881_qi75679</t>
+  </si>
+  <si>
+    <t>DB_A46E6D_sponsor</t>
+  </si>
+  <si>
+    <t>DB_A46E6D_pms</t>
+  </si>
+  <si>
+    <t>DB_A46E6D_admin</t>
+  </si>
+  <si>
+    <t>sql6002.site4now.net</t>
+  </si>
+  <si>
+    <t>DB_A46E6D_Sponsor_admin</t>
+  </si>
+  <si>
+    <t>DB_A46E6D_pms_admin</t>
+  </si>
+  <si>
+    <t>DB_A46E6D_Admin_admin</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=sql6002.site4now.net;UID=m314alta;PWD=Maine1953;APP=Microsoft Office;DATABASE=DB_A46E6D_PMSTest;</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=sql6002.site4now.net;UID=m314alta;PWD=Maine1953;APP=Microsoft Office;DATABASE=DB_A46E6D_PMS;</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=sql6002.site4now.net;UID=m314alta;PWD=Maine1953;APP=Microsoft Office;DATABASE=DB_A46E6D_Sponsor;</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=sql6002.site4now.net;UID=m314alta;PWD=Maine1953;APP=Microsoft Office;DATABASE=DB_A46E6D_Admin;</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=sql6002.site4now.net;UID=m314alta;PWD=Maine1953;APP=Microsoft Office;DATABASE=DB_A46E6D_AdminTest;</t>
+  </si>
+  <si>
+    <t>AdminMember</t>
+  </si>
+  <si>
+    <t>crew</t>
+  </si>
+  <si>
+    <t>PMSMember</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,11 +228,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -493,19 +551,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4541937-B5CE-4A20-80A9-B8C27113714F}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
@@ -515,26 +573,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -686,11 +744,11 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" t="s">
         <v>31</v>
       </c>
@@ -759,9 +817,97 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Utkast versjon 3.4.0 samt PMSTest arbeider
</commit_message>
<xml_diff>
--- a/Source/Navn og passord.xlsx
+++ b/Source/Navn og passord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MaineBoat\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F198B91A-5DBD-45C3-B998-09FF1B1C1178}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DC4A49-8200-4E0E-A8EA-DA428B508665}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
   </bookViews>
@@ -554,7 +554,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K16" sqref="K15:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +669,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1">
         <v>7</v>
@@ -678,7 +678,7 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1">
         <v>5</v>
@@ -687,7 +687,7 @@
         <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J4" s="1">
         <v>3</v>
@@ -696,7 +696,7 @@
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Skiftet server Admin 3.6.0
Div medlemsorienterte rtapporter innført
</commit_message>
<xml_diff>
--- a/Source/Navn og passord.xlsx
+++ b/Source/Navn og passord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MaineBoat\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DC4A49-8200-4E0E-A8EA-DA428B508665}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E221E47-18E2-412C-ACAD-E1B954AF9917}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
+    <workbookView xWindow="13005" yWindow="3255" windowWidth="12735" windowHeight="11835" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K15:K16"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Overføringer til ny Server for alt unntatt Admin (ferdig] og PMS
</commit_message>
<xml_diff>
--- a/Source/Navn og passord.xlsx
+++ b/Source/Navn og passord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MaineBoat\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E221E47-18E2-412C-ACAD-E1B954AF9917}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5020E03F-80EA-494A-A50C-AE0214E06C68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13005" yWindow="3255" windowWidth="12735" windowHeight="11835" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
   </bookViews>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4541937-B5CE-4A20-80A9-B8C27113714F}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Selskap og PVS komp tre
Komptre ferdig, Selskap requeries etter arrangementsdetaljetr
</commit_message>
<xml_diff>
--- a/Source/Navn og passord.xlsx
+++ b/Source/Navn og passord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MaineBoat\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914D1D14-D91D-4F3E-8551-912FE96F4ED6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88950E7D-B284-42E7-A9E7-4167D01E6FD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
+    <workbookView xWindow="8400" yWindow="3765" windowWidth="18735" windowHeight="11835" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Eier</t>
   </si>
@@ -169,6 +169,21 @@
   </si>
   <si>
     <t>M314Sponsor</t>
+  </si>
+  <si>
+    <t>105881_xj61802</t>
+  </si>
+  <si>
+    <t>pvs-105881.mssql.stwcp.net</t>
+  </si>
+  <si>
+    <t>105881_ah72261</t>
+  </si>
+  <si>
+    <t>M314PVS</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=pvs-105881.mssql.stwcp.net;UID=105881-ah72261;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-pvs;</t>
   </si>
 </sst>
 </file>
@@ -313,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -357,6 +372,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4541937-B5CE-4A20-80A9-B8C27113714F}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,38 +992,126 @@
       </c>
       <c r="J10" s="15"/>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="27"/>
+    </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="27"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="27"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="12">
+        <v>9</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H16" t="s">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="K18" t="s">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ver 4.0.0 første del
Ny kompetansedberegning og struktur
</commit_message>
<xml_diff>
--- a/Source/Navn og passord.xlsx
+++ b/Source/Navn og passord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerha\Documents\MaineBoat\Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MaineBoat\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95D5EE6-CE61-48B3-880C-16122C0B9CBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C25514-2447-48BB-A2A4-C2931395A7FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="2604" windowWidth="17280" windowHeight="9024" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -742,26 +742,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4541937-B5CE-4A20-80A9-B8C27113714F}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="1"/>
-    <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
     <col min="11" max="11" width="34" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="2"/>
+    <col min="13" max="13" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -799,7 +799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
         <v>40</v>
       </c>
@@ -821,7 +821,7 @@
       <c r="L2" s="16"/>
       <c r="M2" s="17"/>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
         <v>36</v>
       </c>
@@ -843,7 +843,7 @@
       <c r="L3" s="18"/>
       <c r="M3" s="19"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -876,7 +876,7 @@
       </c>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -917,7 +917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -950,7 +950,7 @@
       </c>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>41</v>
       </c>
@@ -968,7 +968,7 @@
       <c r="J7" s="7"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>22</v>
       </c>
@@ -985,7 +985,7 @@
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="J10" s="15"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="27"/>
@@ -1056,7 +1056,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="27"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="27"/>
@@ -1069,7 +1069,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="27"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="27"/>
@@ -1084,7 +1084,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="27"/>
     </row>
-    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="27"/>
@@ -1101,7 +1101,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="27"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="27"/>
@@ -1114,7 +1114,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="27"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="27"/>
@@ -1127,7 +1127,7 @@
       <c r="I16" s="11"/>
       <c r="J16" s="27"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="27"/>
@@ -1142,7 +1142,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="27"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="27"/>
@@ -1159,7 +1159,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="27"/>
@@ -1170,27 +1170,27 @@
       <c r="I19" s="11"/>
       <c r="J19" s="27"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D25" s="2"/>
       <c r="E25" t="s">
         <v>51</v>
@@ -1198,7 +1198,7 @@
       <c r="G25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
       <c r="E26" t="s">
         <v>56</v>
@@ -1206,17 +1206,17 @@
       <c r="G26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K29" t="s">
         <v>34</v>
       </c>

</xml_diff>